<commit_message>
Simulation files are edited and adjusted to work with changes in other codes
</commit_message>
<xml_diff>
--- a/simulation/shock.xlsx
+++ b/simulation/shock.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="matrix" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="23">
   <si>
     <t>Final uses</t>
   </si>
@@ -81,7 +81,10 @@
     <t>Value</t>
   </si>
   <si>
-    <t>FU</t>
+    <t>Final consumption expenditure of households</t>
+  </si>
+  <si>
+    <t>FCH</t>
   </si>
 </sst>
 </file>
@@ -662,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,10 +722,10 @@
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="4" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -733,10 +736,10 @@
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -759,7 +762,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="15" t="str">
-        <f>B8&amp;D8</f>
+        <f t="shared" ref="H8:H15" si="0">B8&amp;D8</f>
         <v>EU27P1</v>
       </c>
       <c r="I8" s="10"/>
@@ -784,7 +787,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="15" t="str">
-        <f>B9&amp;D9</f>
+        <f t="shared" si="0"/>
         <v>EU27P2</v>
       </c>
       <c r="I9" s="10"/>
@@ -809,7 +812,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="15" t="str">
-        <f>B10&amp;D10</f>
+        <f t="shared" si="0"/>
         <v>EU27P3</v>
       </c>
       <c r="I10" s="10"/>
@@ -834,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="15" t="str">
-        <f>B11&amp;D11</f>
+        <f t="shared" si="0"/>
         <v>EU27P4</v>
       </c>
       <c r="I11" s="10"/>
@@ -859,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="15" t="str">
-        <f>B12&amp;D12</f>
+        <f t="shared" si="0"/>
         <v>USP1</v>
       </c>
       <c r="I12" s="10"/>
@@ -884,7 +887,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="15" t="str">
-        <f>B13&amp;D13</f>
+        <f t="shared" si="0"/>
         <v>USP2</v>
       </c>
       <c r="I13" s="10"/>
@@ -909,7 +912,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="15" t="str">
-        <f>B14&amp;D14</f>
+        <f t="shared" si="0"/>
         <v>USP3</v>
       </c>
       <c r="I14" s="10"/>
@@ -934,7 +937,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="15" t="str">
-        <f>B15&amp;D15</f>
+        <f t="shared" si="0"/>
         <v>USP4</v>
       </c>
       <c r="I15" s="10"/>
@@ -942,11 +945,11 @@
     <row r="17" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E17" s="14" t="str">
         <f>E5&amp;E7</f>
-        <v>EU27FU</v>
+        <v>EU27FCH</v>
       </c>
       <c r="F17" s="14" t="str">
-        <f t="shared" ref="F17" si="0">F5&amp;F7</f>
-        <v>USFU</v>
+        <f t="shared" ref="F17" si="1">F5&amp;F7</f>
+        <v>USFCH</v>
       </c>
     </row>
     <row r="18" spans="5:9" x14ac:dyDescent="0.25">
@@ -972,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,7 +1009,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E2">
         <f ca="1">OFFSET(matrix!$E$8,MATCH(long!A2&amp;long!B2,matrix!$H$8:$H$15,0)-1,MATCH(long!C2&amp;long!D2,matrix!$E$17:$F$17,0)-1)</f>
@@ -1024,7 +1027,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E3">
         <f ca="1">OFFSET(matrix!$E$8,MATCH(long!A3&amp;long!B3,matrix!$H$8:$H$15,0)-1,MATCH(long!C3&amp;long!D3,matrix!$E$17:$F$17,0)-1)</f>
@@ -1042,7 +1045,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4">
         <f ca="1">OFFSET(matrix!$E$8,MATCH(long!A4&amp;long!B4,matrix!$H$8:$H$15,0)-1,MATCH(long!C4&amp;long!D4,matrix!$E$17:$F$17,0)-1)</f>
@@ -1060,7 +1063,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5">
         <f ca="1">OFFSET(matrix!$E$8,MATCH(long!A5&amp;long!B5,matrix!$H$8:$H$15,0)-1,MATCH(long!C5&amp;long!D5,matrix!$E$17:$F$17,0)-1)</f>
@@ -1078,7 +1081,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6">
         <f ca="1">OFFSET(matrix!$E$8,MATCH(long!A6&amp;long!B6,matrix!$H$8:$H$15,0)-1,MATCH(long!C6&amp;long!D6,matrix!$E$17:$F$17,0)-1)</f>
@@ -1096,7 +1099,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E7">
         <f ca="1">OFFSET(matrix!$E$8,MATCH(long!A7&amp;long!B7,matrix!$H$8:$H$15,0)-1,MATCH(long!C7&amp;long!D7,matrix!$E$17:$F$17,0)-1)</f>
@@ -1114,7 +1117,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E8">
         <f ca="1">OFFSET(matrix!$E$8,MATCH(long!A8&amp;long!B8,matrix!$H$8:$H$15,0)-1,MATCH(long!C8&amp;long!D8,matrix!$E$17:$F$17,0)-1)</f>
@@ -1132,7 +1135,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E9">
         <f ca="1">OFFSET(matrix!$E$8,MATCH(long!A9&amp;long!B9,matrix!$H$8:$H$15,0)-1,MATCH(long!C9&amp;long!D9,matrix!$E$17:$F$17,0)-1)</f>
@@ -1150,7 +1153,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E10">
         <f ca="1">OFFSET(matrix!$E$8,MATCH(long!A10&amp;long!B10,matrix!$H$8:$H$15,0)-1,MATCH(long!C10&amp;long!D10,matrix!$E$17:$F$17,0)-1)</f>
@@ -1168,7 +1171,7 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E11">
         <f ca="1">OFFSET(matrix!$E$8,MATCH(long!A11&amp;long!B11,matrix!$H$8:$H$15,0)-1,MATCH(long!C11&amp;long!D11,matrix!$E$17:$F$17,0)-1)</f>
@@ -1186,7 +1189,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E12">
         <f ca="1">OFFSET(matrix!$E$8,MATCH(long!A12&amp;long!B12,matrix!$H$8:$H$15,0)-1,MATCH(long!C12&amp;long!D12,matrix!$E$17:$F$17,0)-1)</f>
@@ -1204,7 +1207,7 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E13">
         <f ca="1">OFFSET(matrix!$E$8,MATCH(long!A13&amp;long!B13,matrix!$H$8:$H$15,0)-1,MATCH(long!C13&amp;long!D13,matrix!$E$17:$F$17,0)-1)</f>
@@ -1222,7 +1225,7 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E14">
         <f ca="1">OFFSET(matrix!$E$8,MATCH(long!A14&amp;long!B14,matrix!$H$8:$H$15,0)-1,MATCH(long!C14&amp;long!D14,matrix!$E$17:$F$17,0)-1)</f>
@@ -1240,7 +1243,7 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E15">
         <f ca="1">OFFSET(matrix!$E$8,MATCH(long!A15&amp;long!B15,matrix!$H$8:$H$15,0)-1,MATCH(long!C15&amp;long!D15,matrix!$E$17:$F$17,0)-1)</f>
@@ -1258,7 +1261,7 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E16">
         <f ca="1">OFFSET(matrix!$E$8,MATCH(long!A16&amp;long!B16,matrix!$H$8:$H$15,0)-1,MATCH(long!C16&amp;long!D16,matrix!$E$17:$F$17,0)-1)</f>
@@ -1276,7 +1279,7 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E17">
         <f ca="1">OFFSET(matrix!$E$8,MATCH(long!A17&amp;long!B17,matrix!$H$8:$H$15,0)-1,MATCH(long!C17&amp;long!D17,matrix!$E$17:$F$17,0)-1)</f>

</xml_diff>